<commit_message>
Adicion del caso alterno y refactorizacion - Pendiente detalle de tres objetos
</commit_message>
<xml_diff>
--- a/bin/datadrivens/DDReto.xlsx
+++ b/bin/datadrivens/DDReto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Orientacion</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Carlos B.</t>
   </si>
   <si>
-    <t>Jorge H.</t>
-  </si>
-  <si>
     <t>Morata</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>ckariues</t>
   </si>
   <si>
-    <t>jsanchez</t>
-  </si>
-  <si>
     <t>rramirez</t>
   </si>
   <si>
@@ -142,6 +136,21 @@
   </si>
   <si>
     <t>Datos guardados correctamente.</t>
+  </si>
+  <si>
+    <t>Cita Error</t>
+  </si>
+  <si>
+    <t>juribe</t>
+  </si>
+  <si>
+    <t>Uribe</t>
+  </si>
+  <si>
+    <t>20/06/2018</t>
+  </si>
+  <si>
+    <t>Error:</t>
   </si>
 </sst>
 </file>
@@ -531,7 +540,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,19 +565,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -576,25 +585,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -602,26 +611,36 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -640,7 +659,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +673,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -663,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -674,7 +693,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -694,7 +713,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -706,7 +725,7 @@
         <v>3267788</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3">
         <v>102131</v>
@@ -714,7 +733,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
@@ -729,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="3">
-        <v>102232</v>
+        <v>10299990</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +762,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +773,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -766,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -774,13 +793,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -794,19 +813,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4">
         <v>102131</v>
@@ -814,22 +833,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="4">
-        <v>3206522929</v>
+        <v>1010198</v>
       </c>
       <c r="F4" s="4">
-        <v>102232</v>
+        <v>10001009</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>